<commit_message>
manual dislocation uploading 2021/07/19 13:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/KBL.xlsx
+++ b/src/algorithms/plan_fact_module/KBL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>